<commit_message>
first try adapting openEmpire to new model
</commit_message>
<xml_diff>
--- a/EMPIRE_extension/EMPIRE_input/General.xlsx
+++ b/EMPIRE_extension/EMPIRE_input/General.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gorandurakovic/EMPIRE-Wind_North_Sea/Data handler/hydrogenAllCountries/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/stianbac_ntnu_no/Documents/EMPIRE/EMPIRE in Pyomo/EMPIRE-Pyomo/Data handler/europe_v50/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D11A978-46E9-DC43-AFBC-6D8E01739837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{8CEA8F0B-1B7F-448F-9B1D-D4F277756DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2080" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="seasonScale" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="nodeLostLoadCost">#REF!</definedName>
     <definedName name="seaScale">seasonScale!$A$3:$B$9</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,6 +36,8 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,7 +47,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
+    <t>Source: Assumed</t>
+  </si>
+  <si>
+    <t>Description: The annual scaling of each representative season (one representative season repeats X times in one year)</t>
+  </si>
+  <si>
     <t>Season</t>
+  </si>
+  <si>
+    <t>seasonScale</t>
   </si>
   <si>
     <t>winter</t>
@@ -66,22 +77,16 @@
     <t>peak2</t>
   </si>
   <si>
-    <t>seasonScale</t>
+    <t xml:space="preserve">Source: A Clean Planet for all A European strategic long-term vision for a prosperous, modern, competitive and climate neutral economy </t>
   </si>
   <si>
-    <t>Source: Assumed</t>
-  </si>
-  <si>
-    <t>Description: The annual scaling of each representative season (one representative season repeats X times in one year)</t>
+    <t>Description: Maximum allowed annual emissions for investment period</t>
   </si>
   <si>
     <t>Period</t>
   </si>
   <si>
-    <t>CO2price in euro per tCO2</t>
-  </si>
-  <si>
-    <t>Description: Maximum allowed annual emissions for investment period</t>
+    <t>CO2Cap [in Mton CO2eq]</t>
   </si>
   <si>
     <t>Source: EC decarb reference scenario</t>
@@ -90,17 +95,14 @@
     <t>Description: Assumed price per CO2 from the EU ETS</t>
   </si>
   <si>
-    <t>CO2Cap [in Mton CO2eq]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: A Clean Planet for all A European strategic long-term vision for a prosperous, modern, competitive and climate neutral economy </t>
+    <t>CO2price in euro per tCO2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,7 +191,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-NO"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -306,7 +308,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-NO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="756441551"/>
@@ -365,7 +367,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-NO"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="539877327"/>
@@ -413,7 +415,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-NO"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1028,44 +1030,7 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Nodes</v>
-          </cell>
-          <cell r="B1" t="str">
-            <v>Period</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>Scenario</v>
-          </cell>
-          <cell r="D1" t="str">
-            <v>maxRegHydroNode</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>N1</v>
-          </cell>
-          <cell r="B2">
-            <v>1</v>
-          </cell>
-          <cell r="D2">
-            <v>1000</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>N2</v>
-          </cell>
-          <cell r="B3">
-            <v>1</v>
-          </cell>
-          <cell r="D3">
-            <v>1000</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1336,83 +1301,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <f>(8760-2*24)/(7*24*4)</f>
+        <f>(8760-48)/672</f>
         <v>12.964285714285714</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B7" si="0">(8760-2*24)/(7*24*4)</f>
+        <f t="shared" ref="B5:B7" si="0">(8760-48)/672</f>
         <v>12.964285714285714</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>12.964285714285714</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>12.964285714285714</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1428,34 +1393,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45EF7C0-A682-4EA7-BDB7-45A9075F127B}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
       <c r="B3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1463,7 +1428,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1472,7 +1437,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1481,7 +1446,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1490,7 +1455,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1499,7 +1464,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1508,7 +1473,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1517,7 +1482,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1540,30 +1505,30 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1571,7 +1536,7 @@
         <v>14.285714285714283</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1579,7 +1544,7 @@
         <v>23.80952380952381</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1587,7 +1552,7 @@
         <v>39.999999999999993</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1595,7 +1560,7 @@
         <v>83.80952380952381</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1603,7 +1568,7 @@
         <v>152.38095238095238</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1611,7 +1576,7 @@
         <v>304.76190476190476</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1619,7 +1584,7 @@
         <v>523.80952380952374</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1630,4 +1595,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E6F967323C0D5D438811C071A0F9DCC2" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b27e86270437fbb2bd82bf5c2c3c6393">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d8af0d66-b3db-4c81-87bc-15f9b72a49e2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e49c777b2df3ddef5cddc816a3965e22" ns2:_="">
+    <xsd:import namespace="d8af0d66-b3db-4c81-87bc-15f9b72a49e2"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d8af0d66-b3db-4c81-87bc-15f9b72a49e2" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{109E4AE2-910A-4EBB-95CE-AFD22503F831}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37C661E5-5DF3-46E4-97A2-26023877D29C}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9674C98-65DF-49EF-9E0D-5D63F1B7E3B1}"/>
 </file>
</xml_diff>